<commit_message>
Functionized saving to db
</commit_message>
<xml_diff>
--- a/backend/data/UGCSyllabus.xlsx
+++ b/backend/data/UGCSyllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aditya data\Projects\StudyPlannerApp\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69102D3-B19A-47D5-9B1B-C0DE08ACB0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041F752-E872-4C74-B363-98149280CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,53 +35,53 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>Unit - 8: Family, Marriage &amp; Kinship
-Inheritance, Succession and Authority</t>
-  </si>
-  <si>
-    <t>Partible versus impartible inheritance</t>
-  </si>
-  <si>
-    <t>Primogeniture, ultimogeniture, seniority as succession rules</t>
-  </si>
-  <si>
-    <t>Lineal versus collateral succession</t>
-  </si>
-  <si>
-    <t>Patrilineal, matrilineal, bilateral inheritance patterns across communities</t>
-  </si>
-  <si>
-    <t>Avunculate and succession to sister’s son in matriliny</t>
-  </si>
-  <si>
-    <t>Residence and authority: patrilocal, matrilocal, neolocal effects on decision-making</t>
-  </si>
-  <si>
-    <t>Karta’s role and authority in a joint household</t>
-  </si>
-  <si>
-    <t>Corporate versus self-acquired property control in descent groups</t>
-  </si>
-  <si>
-    <t>Authority by age and generation: gerontocracy and seniority principle</t>
-  </si>
-  <si>
-    <t>Matrilineal authority among Khasi/Garo and the mother’s brother</t>
-  </si>
-  <si>
-    <t>Succession to ritual office (lineage priest/head)</t>
-  </si>
-  <si>
-    <t>Segmentary lineage organization and authority distribution</t>
-  </si>
-  <si>
-    <t>Household decision rules: patriarchal veto, consensus, seniority</t>
-  </si>
-  <si>
-    <t>Kin role obligations (mother’s brother versus father) and authority expectations</t>
-  </si>
-  <si>
-    <t>Tribal chiefship succession: hereditary versus elective</t>
+    <t>Unit - 9 : Science, Technology &amp; Society
+Technology and Emerging Political Processes, State Policy, Digital Divide and Inclusion</t>
+  </si>
+  <si>
+    <t>Networked social movements and connective action (Castells; Bennett and Segerberg)</t>
+  </si>
+  <si>
+    <t>Hashtag activism versus slacktivism</t>
+  </si>
+  <si>
+    <t>Computational propaganda, bots, and astroturfing (Philip N. Howard)</t>
+  </si>
+  <si>
+    <t>Microtargeting and political advertising on platforms</t>
+  </si>
+  <si>
+    <t>E-participation tools: e-petitions, MyGov, online RTI</t>
+  </si>
+  <si>
+    <t>Civic technology and open data for accountability</t>
+  </si>
+  <si>
+    <t>Platform governance and content moderation as political process</t>
+  </si>
+  <si>
+    <t>Internet shutdowns and throttling as digital authoritarian practices</t>
+  </si>
+  <si>
+    <t>Data localization and digital sovereignty</t>
+  </si>
+  <si>
+    <t>Digital divide levels: access, skills, usage, outcome divides</t>
+  </si>
+  <si>
+    <t>Intersectional divides: gender, rural–urban, disability, language</t>
+  </si>
+  <si>
+    <t>Inclusion strategies: BharatNet, CSCs, PMGDISHA, WCAG accessibility</t>
+  </si>
+  <si>
+    <t>Assistive technology and inclusive design: screen readers, captions, UPI 123PAY</t>
+  </si>
+  <si>
+    <t>EVMs and VVPAT: trust, transparency, auditability debates</t>
+  </si>
+  <si>
+    <t>Platform/gig workers’ collective action and algorithmic bargaining</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -184,9 +184,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -204,6 +201,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,7 +714,7 @@
   <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection sqref="A1:A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.95" customHeight="1"/>
@@ -705,7 +723,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
@@ -716,7 +734,7 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
@@ -727,7 +745,7 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
@@ -738,7 +756,7 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
@@ -749,7 +767,7 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
@@ -760,7 +778,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3"/>
@@ -772,7 +790,7 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
@@ -782,10 +800,10 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="11"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
@@ -795,10 +813,10 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="12"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
@@ -808,10 +826,10 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="13"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
@@ -821,10 +839,10 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="13"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="3"/>
@@ -834,10 +852,10 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="14"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="3"/>
@@ -850,7 +868,7 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="3"/>
@@ -863,7 +881,7 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
@@ -876,7 +894,7 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
@@ -887,7 +905,7 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="13.95" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3"/>
@@ -898,249 +916,274 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A17" s="14"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A18" s="14"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A19" s="14"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A20" s="14"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A21" s="14"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A22" s="14"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A23" s="14"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A24" s="7"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A25" s="8"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A26" s="14"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A27" s="14"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A28" s="14"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A29" s="14"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A30" s="14"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A31" s="7"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A32" s="7"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A33" s="7"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A34" s="7"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A35" s="7"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A36" s="7"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A37" s="8"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A38" s="16"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A39" s="16"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A40" s="16"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A41" s="18"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A42" s="16"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A43" s="7"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A44" s="7"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A45" s="7"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A46" s="7"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A47" s="7"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A48" s="7"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A49" s="8"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A50" s="16"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A51" s="16"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A52" s="16"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A53" s="16"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A54" s="16"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A55" s="16"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
     <row r="56" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A56" s="16"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A57" s="17"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -1148,13 +1191,15 @@
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A58" s="17"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
-      <c r="E58" s="10"/>
+      <c r="E58" s="9"/>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A59" s="17"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -1162,208 +1207,272 @@
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A60" s="18"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A61" s="16"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A62" s="16"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A63" s="16"/>
       <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A64" s="16"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" spans="5:6" ht="13.95" customHeight="1">
+    <row r="65" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A65" s="14"/>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" spans="5:6" ht="13.95" customHeight="1">
+    <row r="66" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A66" s="14"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="5:6" ht="13.95" customHeight="1">
+    <row r="67" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A67" s="14"/>
       <c r="E67" s="6"/>
     </row>
-    <row r="68" spans="5:6" ht="13.95" customHeight="1">
+    <row r="68" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A68" s="14"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="5:6" ht="13.95" customHeight="1">
+    <row r="69" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A69" s="14"/>
       <c r="E69" s="6"/>
     </row>
-    <row r="70" spans="5:6" ht="13.95" customHeight="1">
+    <row r="70" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A70" s="14"/>
       <c r="E70" s="6"/>
     </row>
-    <row r="71" spans="5:6" ht="13.95" customHeight="1">
+    <row r="71" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A71" s="14"/>
       <c r="E71" s="6"/>
     </row>
-    <row r="72" spans="5:6" ht="13.95" customHeight="1">
+    <row r="72" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A72" s="14"/>
       <c r="E72" s="6"/>
     </row>
-    <row r="73" spans="5:6" ht="13.95" customHeight="1">
+    <row r="73" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A73" s="14"/>
       <c r="E73" s="6"/>
     </row>
-    <row r="74" spans="5:6" ht="13.95" customHeight="1">
+    <row r="74" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A74" s="14"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="5:6" ht="13.95" customHeight="1">
+    <row r="75" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A75" s="14"/>
       <c r="E75" s="6"/>
     </row>
-    <row r="76" spans="5:6" ht="13.95" customHeight="1">
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-    </row>
-    <row r="77" spans="5:6" ht="13.95" customHeight="1">
+    <row r="76" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A76" s="18"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+    </row>
+    <row r="77" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A77" s="14"/>
       <c r="E77" s="6"/>
     </row>
-    <row r="78" spans="5:6" ht="13.95" customHeight="1">
+    <row r="78" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A78" s="14"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="5:6" ht="13.95" customHeight="1">
+    <row r="79" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A79" s="14"/>
       <c r="E79" s="6"/>
     </row>
-    <row r="80" spans="5:6" ht="13.95" customHeight="1">
+    <row r="80" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A80" s="14"/>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="5:6" ht="13.95" customHeight="1">
+    <row r="81" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A81" s="14"/>
       <c r="E81" s="6"/>
     </row>
-    <row r="82" spans="5:6" ht="13.95" customHeight="1">
+    <row r="82" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A82" s="14"/>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="5:6" ht="13.95" customHeight="1">
+    <row r="83" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A83" s="14"/>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" spans="5:6" ht="13.95" customHeight="1">
+    <row r="84" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A84" s="14"/>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" spans="5:6" ht="13.95" customHeight="1">
+    <row r="85" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A85" s="14"/>
       <c r="E85" s="6"/>
     </row>
-    <row r="86" spans="5:6" ht="13.95" customHeight="1">
+    <row r="86" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A86" s="14"/>
       <c r="E86" s="6"/>
     </row>
-    <row r="87" spans="5:6" ht="13.95" customHeight="1">
+    <row r="87" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A87" s="14"/>
       <c r="E87" s="6"/>
     </row>
-    <row r="88" spans="5:6" ht="13.95" customHeight="1">
+    <row r="88" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A88" s="14"/>
       <c r="E88" s="6"/>
     </row>
-    <row r="89" spans="5:6" ht="13.95" customHeight="1">
+    <row r="89" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A89" s="14"/>
       <c r="E89" s="6"/>
     </row>
-    <row r="90" spans="5:6" ht="13.95" customHeight="1">
+    <row r="90" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A90" s="14"/>
       <c r="E90" s="6"/>
     </row>
-    <row r="91" spans="5:6" ht="13.95" customHeight="1">
+    <row r="91" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A91" s="14"/>
       <c r="E91" s="6"/>
     </row>
-    <row r="92" spans="5:6" ht="13.95" customHeight="1">
-      <c r="E92" s="9"/>
-      <c r="F92" s="9"/>
-    </row>
-    <row r="93" spans="5:6" ht="13.95" customHeight="1">
+    <row r="92" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A92" s="18"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A93" s="14"/>
       <c r="E93" s="6"/>
     </row>
-    <row r="94" spans="5:6" ht="13.95" customHeight="1">
+    <row r="94" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A94" s="14"/>
       <c r="E94" s="6"/>
     </row>
-    <row r="95" spans="5:6" ht="13.95" customHeight="1">
+    <row r="95" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A95" s="14"/>
       <c r="E95" s="6"/>
     </row>
-    <row r="96" spans="5:6" ht="13.95" customHeight="1">
+    <row r="96" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A96" s="14"/>
       <c r="E96" s="6"/>
     </row>
-    <row r="97" spans="5:6" ht="13.95" customHeight="1">
+    <row r="97" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A97" s="14"/>
       <c r="E97" s="6"/>
     </row>
-    <row r="98" spans="5:6" ht="13.95" customHeight="1">
+    <row r="98" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A98" s="14"/>
       <c r="E98" s="6"/>
     </row>
-    <row r="99" spans="5:6" ht="13.95" customHeight="1">
+    <row r="99" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A99" s="14"/>
       <c r="E99" s="6"/>
     </row>
-    <row r="100" spans="5:6" ht="13.95" customHeight="1">
+    <row r="100" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A100" s="14"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="5:6" ht="13.95" customHeight="1">
+    <row r="101" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A101" s="14"/>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="5:6" ht="13.95" customHeight="1">
+    <row r="102" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A102" s="14"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="5:6" ht="13.95" customHeight="1">
+    <row r="103" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A103" s="14"/>
       <c r="E103" s="6"/>
     </row>
-    <row r="104" spans="5:6" ht="13.95" customHeight="1">
+    <row r="104" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A104" s="14"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="5:6" ht="13.95" customHeight="1">
+    <row r="105" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A105" s="14"/>
       <c r="E105" s="6"/>
     </row>
-    <row r="106" spans="5:6" ht="13.95" customHeight="1">
+    <row r="106" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A106" s="14"/>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="5:6" ht="13.95" customHeight="1">
+    <row r="107" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A107" s="14"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="5:6" ht="13.95" customHeight="1">
-      <c r="E108" s="9"/>
-      <c r="F108" s="9"/>
-    </row>
-    <row r="109" spans="5:6" ht="13.95" customHeight="1">
+    <row r="108" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A108" s="18"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+    </row>
+    <row r="109" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A109" s="14"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="5:6" ht="13.95" customHeight="1">
+    <row r="110" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A110" s="14"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="5:6" ht="13.95" customHeight="1">
+    <row r="111" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A111" s="14"/>
       <c r="E111" s="6"/>
     </row>
-    <row r="112" spans="5:6" ht="13.95" customHeight="1">
+    <row r="112" spans="1:6" ht="13.95" customHeight="1">
+      <c r="A112" s="14"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="5:5" ht="13.95" customHeight="1">
+    <row r="113" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A113" s="14"/>
       <c r="E113" s="6"/>
     </row>
-    <row r="114" spans="5:5" ht="13.95" customHeight="1">
+    <row r="114" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A114" s="14"/>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="5:5" ht="13.95" customHeight="1">
+    <row r="115" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A115" s="14"/>
       <c r="E115" s="6"/>
     </row>
-    <row r="116" spans="5:5" ht="13.95" customHeight="1">
+    <row r="116" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A116" s="14"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="5:5" ht="13.95" customHeight="1">
+    <row r="117" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A117" s="14"/>
       <c r="E117" s="6"/>
     </row>
-    <row r="118" spans="5:5" ht="13.95" customHeight="1">
+    <row r="118" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A118" s="14"/>
       <c r="E118" s="6"/>
     </row>
-    <row r="119" spans="5:5" ht="13.95" customHeight="1">
+    <row r="119" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A119" s="14"/>
       <c r="E119" s="6"/>
     </row>
-    <row r="120" spans="5:5" ht="13.95" customHeight="1">
+    <row r="120" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A120" s="14"/>
       <c r="E120" s="6"/>
     </row>
-    <row r="121" spans="5:5" ht="13.95" customHeight="1">
+    <row r="121" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A121" s="14"/>
       <c r="E121" s="6"/>
     </row>
-    <row r="122" spans="5:5" ht="13.95" customHeight="1">
+    <row r="122" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A122" s="14"/>
       <c r="E122" s="6"/>
     </row>
-    <row r="123" spans="5:5" ht="13.95" customHeight="1">
+    <row r="123" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A123" s="14"/>
       <c r="E123" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Let the User add the Syllabus
</commit_message>
<xml_diff>
--- a/backend/data/UGCSyllabus.xlsx
+++ b/backend/data/UGCSyllabus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aditya data\Projects\StudyPlannerApp\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041F752-E872-4C74-B363-98149280CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D177A6F-6FA3-476E-B6AA-7F13BEA91410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,60 +35,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>Unit - 9 : Science, Technology &amp; Society
-Technology and Emerging Political Processes, State Policy, Digital Divide and Inclusion</t>
-  </si>
-  <si>
-    <t>Networked social movements and connective action (Castells; Bennett and Segerberg)</t>
-  </si>
-  <si>
-    <t>Hashtag activism versus slacktivism</t>
-  </si>
-  <si>
-    <t>Computational propaganda, bots, and astroturfing (Philip N. Howard)</t>
-  </si>
-  <si>
-    <t>Microtargeting and political advertising on platforms</t>
-  </si>
-  <si>
-    <t>E-participation tools: e-petitions, MyGov, online RTI</t>
-  </si>
-  <si>
-    <t>Civic technology and open data for accountability</t>
-  </si>
-  <si>
-    <t>Platform governance and content moderation as political process</t>
-  </si>
-  <si>
-    <t>Internet shutdowns and throttling as digital authoritarian practices</t>
-  </si>
-  <si>
-    <t>Data localization and digital sovereignty</t>
-  </si>
-  <si>
-    <t>Digital divide levels: access, skills, usage, outcome divides</t>
-  </si>
-  <si>
-    <t>Intersectional divides: gender, rural–urban, disability, language</t>
-  </si>
-  <si>
-    <t>Inclusion strategies: BharatNet, CSCs, PMGDISHA, WCAG accessibility</t>
-  </si>
-  <si>
-    <t>Assistive technology and inclusive design: screen readers, captions, UPI 123PAY</t>
-  </si>
-  <si>
-    <t>EVMs and VVPAT: trust, transparency, auditability debates</t>
-  </si>
-  <si>
-    <t>Platform/gig workers’ collective action and algorithmic bargaining</t>
+    <t>Unit - 10 : Culture &amp; Symbolic Transformations
+Culture, Politics &amp; Environment
+Culture and Environment, Culture and Politics, Sports and Culture</t>
+  </si>
+  <si>
+    <t>Political ecology and environmental justice</t>
+  </si>
+  <si>
+    <t>Indigenous knowledge systems and conservation</t>
+  </si>
+  <si>
+    <t>Climate change, risk perception, and adaptation</t>
+  </si>
+  <si>
+    <t>Development projects, displacement, and resistance</t>
+  </si>
+  <si>
+    <t>Environmental movements: Chipko to Narmada Bachao Andolan</t>
+  </si>
+  <si>
+    <t>Ecofeminism and gendered environmental labor</t>
+  </si>
+  <si>
+    <t>Cultural values, religion, and environmental stewardship</t>
+  </si>
+  <si>
+    <t>Urban environmentalism and middle-class activism</t>
+  </si>
+  <si>
+    <t>Media framings of environment and disaster</t>
+  </si>
+  <si>
+    <t>Culture, nationalism, and sports mega-events</t>
+  </si>
+  <si>
+    <t>Sports, identity politics, and social stratification</t>
+  </si>
+  <si>
+    <t>Doping, commercialization, and ethics in sport</t>
+  </si>
+  <si>
+    <t>Antonio Gramsci’s hegemony and cultural politics</t>
+  </si>
+  <si>
+    <t>Bruno Latour’s Politics of Nature and political ecology</t>
+  </si>
+  <si>
+    <t>Vandana Shiva’s Monocultures of the Mind and environmentalism</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +137,17 @@
       <name val="Inter"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -205,23 +217,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,7 +726,7 @@
   <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection sqref="A1:A123"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.95" customHeight="1"/>
@@ -916,161 +928,161 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A17" s="14"/>
+      <c r="A17" s="18"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A18" s="14"/>
+      <c r="A18" s="18"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A19" s="14"/>
+      <c r="A19" s="18"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A20" s="14"/>
+      <c r="A20" s="18"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A21" s="14"/>
+      <c r="A21" s="18"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A22" s="14"/>
+      <c r="A22" s="18"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A23" s="14"/>
+      <c r="A23" s="18"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A24" s="14"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A25" s="15"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A26" s="14"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A27" s="14"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A28" s="14"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A29" s="14"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A30" s="14"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A31" s="14"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A32" s="14"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A33" s="16"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A34" s="16"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A35" s="16"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A36" s="16"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A37" s="16"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A38" s="16"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A39" s="16"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A40" s="16"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A41" s="18"/>
+      <c r="A41" s="17"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1078,112 +1090,112 @@
       <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A42" s="16"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A43" s="16"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A44" s="16"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A45" s="16"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A46" s="16"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A47" s="16"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A48" s="16"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A49" s="16"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A50" s="16"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A51" s="16"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A52" s="16"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A53" s="16"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A54" s="16"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A55" s="16"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
     <row r="56" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A56" s="16"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A57" s="17"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -1191,7 +1203,7 @@
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A58" s="17"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -1199,7 +1211,7 @@
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A59" s="17"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -1207,7 +1219,7 @@
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A60" s="18"/>
+      <c r="A60" s="17"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -1215,25 +1227,25 @@
       <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A61" s="16"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A62" s="16"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A63" s="16"/>
+      <c r="A63" s="15"/>
       <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A64" s="16"/>
+      <c r="A64" s="15"/>
       <c r="E64" s="6"/>
     </row>
     <row r="65" spans="1:6" ht="13.95" customHeight="1">
@@ -1281,7 +1293,7 @@
       <c r="E75" s="6"/>
     </row>
     <row r="76" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A76" s="18"/>
+      <c r="A76" s="17"/>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
     </row>
@@ -1346,7 +1358,7 @@
       <c r="E91" s="6"/>
     </row>
     <row r="92" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A92" s="18"/>
+      <c r="A92" s="17"/>
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
     </row>
@@ -1411,7 +1423,7 @@
       <c r="E107" s="6"/>
     </row>
     <row r="108" spans="1:6" ht="13.95" customHeight="1">
-      <c r="A108" s="18"/>
+      <c r="A108" s="17"/>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
     </row>

</xml_diff>